<commit_message>
Updated Assets.xlsx with Necromancer Standing and Sitting
</commit_message>
<xml_diff>
--- a/assets/AssetDB.xlsx
+++ b/assets/AssetDB.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A200274772\GitHub\Crawler-Projektpraktikum\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A200274089\dev\projects\Uni\5.SemesterProjekt\Crawler-Projektpraktikum\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F214C6-8587-4824-8FB1-B6DBAE7079DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648EA484-B657-441B-BBCF-F795A587A9E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{B3F5CE5B-25EC-484D-8705-D10708A494B7}"/>
   </bookViews>
@@ -40,7 +40,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="39">
+  <futureMetadata name="XLRICHVALUE" count="41">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -314,8 +314,22 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="39"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="40"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="39">
+  <valueMetadata count="41">
     <bk>
       <rc t="1" v="0"/>
     </bk>
@@ -432,13 +446,19 @@
     </bk>
     <bk>
       <rc t="1" v="38"/>
+    </bk>
+    <bk>
+      <rc t="1" v="39"/>
+    </bk>
+    <bk>
+      <rc t="1" v="40"/>
     </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="67">
   <si>
     <t>Category</t>
   </si>
@@ -627,6 +647,18 @@
   </si>
   <si>
     <t>safe_marker.png</t>
+  </si>
+  <si>
+    <t>Endboss</t>
+  </si>
+  <si>
+    <t>Necromancer-Standing.png</t>
+  </si>
+  <si>
+    <t>Map Tile/ Endboss</t>
+  </si>
+  <si>
+    <t>Necromancer-Sitting.png</t>
   </si>
 </sst>
 </file>
@@ -908,8 +940,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="7">
     <dxf>
@@ -1174,7 +1206,7 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="39">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="41">
   <rv s="0">
     <v>0</v>
     <v>5</v>
@@ -1329,6 +1361,14 @@
   </rv>
   <rv s="0">
     <v>38</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>39</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>40</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -1384,6 +1424,8 @@
   <rel r:id="rId37"/>
   <rel r:id="rId38"/>
   <rel r:id="rId39"/>
+  <rel r:id="rId40"/>
+  <rel r:id="rId41"/>
 </richValueRels>
 </file>
 
@@ -1401,7 +1443,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1719,11 +1761,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D18B40B6-A108-4343-8456-7741D8A067D3}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="93" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.5546875" bestFit="1" customWidth="1"/>
@@ -2312,16 +2354,32 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="10"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="10"/>
+      <c r="A43" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="2" t="e" vm="40">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="2" t="e" vm="41">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>

</xml_diff>